<commit_message>
remove inflation rounding issue
</commit_message>
<xml_diff>
--- a/excel/2/Inflation.xlsx
+++ b/excel/2/Inflation.xlsx
@@ -5,30 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/github/benofben/the_intelligent_property_investor/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/github/benofben/the_intelligent_property_investor/excel/2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{154E22C3-091E-9447-886A-088C4E33EBB9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{154E22C3-091E-9447-886A-088C4E33EBB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$104</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$2:$C$104</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$104</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$104</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$2:$A$104</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$104</definedName>
-  </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -93,10 +79,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,316 +1194,316 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$104</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="103"/>
                 <c:pt idx="0">
-                  <c:v>3.2912621359223286E-2</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2899999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2620,7 +2607,7 @@
   <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2643,1134 +2630,1133 @@
       <c r="A2">
         <v>1914</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.01</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(B2:B104)</f>
-        <v>3.2912621359223286E-2</v>
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1915</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.01</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.03</v>
+      <c r="C3" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1916</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.08</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.03</v>
+      <c r="C4" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1917</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.17</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.03</v>
+      <c r="C5" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1918</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.18</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.03</v>
+      <c r="C6" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1919</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.15</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.03</v>
+      <c r="C7" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1920</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.16</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.03</v>
+      <c r="C8" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1921</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>-0.11</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.03</v>
+      <c r="C9" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1922</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>-0.06</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.03</v>
+      <c r="C10" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1923</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0.02</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.03</v>
+      <c r="C11" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1924</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.03</v>
+      <c r="C12" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1925</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>0.02</v>
       </c>
-      <c r="C13" s="1">
-        <v>0.03</v>
+      <c r="C13" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1926</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>0.01</v>
       </c>
-      <c r="C14" s="1">
-        <v>0.03</v>
+      <c r="C14" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1927</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>-0.02</v>
       </c>
-      <c r="C15" s="1">
-        <v>0.03</v>
+      <c r="C15" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1928</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>-0.02</v>
       </c>
-      <c r="C16" s="1">
-        <v>0.03</v>
+      <c r="C16" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1929</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
-        <v>0.03</v>
+      <c r="C17" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1930</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>-0.02</v>
       </c>
-      <c r="C18" s="1">
-        <v>0.03</v>
+      <c r="C18" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1931</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>-0.09</v>
       </c>
-      <c r="C19" s="1">
-        <v>0.03</v>
+      <c r="C19" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1932</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>-0.1</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.03</v>
+      <c r="C20" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1933</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>-0.05</v>
       </c>
-      <c r="C21" s="1">
-        <v>0.03</v>
+      <c r="C21" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1934</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>0.03</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.03</v>
+      <c r="C22" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1935</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>0.02</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.03</v>
+      <c r="C23" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1936</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>0.02</v>
       </c>
-      <c r="C24" s="1">
-        <v>0.03</v>
+      <c r="C24" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1937</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>0.04</v>
       </c>
-      <c r="C25" s="1">
-        <v>0.03</v>
+      <c r="C25" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1938</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>-0.02</v>
       </c>
-      <c r="C26" s="1">
-        <v>0.03</v>
+      <c r="C26" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1939</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>-0.01</v>
       </c>
-      <c r="C27" s="1">
-        <v>0.03</v>
+      <c r="C27" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1940</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>0.01</v>
       </c>
-      <c r="C28" s="1">
-        <v>0.03</v>
+      <c r="C28" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1941</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>0.05</v>
       </c>
-      <c r="C29" s="1">
-        <v>0.03</v>
+      <c r="C29" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1942</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>0.11</v>
       </c>
-      <c r="C30" s="1">
-        <v>0.03</v>
+      <c r="C30" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1943</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>0.06</v>
       </c>
-      <c r="C31" s="1">
-        <v>0.03</v>
+      <c r="C31" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1944</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>0.02</v>
       </c>
-      <c r="C32" s="1">
-        <v>0.03</v>
+      <c r="C32" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1945</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>0.02</v>
       </c>
-      <c r="C33" s="1">
-        <v>0.03</v>
+      <c r="C33" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1946</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>0.08</v>
       </c>
-      <c r="C34" s="1">
-        <v>0.03</v>
+      <c r="C34" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1947</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C35" s="1">
-        <v>0.03</v>
+      <c r="C35" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1948</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>0.08</v>
       </c>
-      <c r="C36" s="1">
-        <v>0.03</v>
+      <c r="C36" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1949</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>-0.01</v>
       </c>
-      <c r="C37" s="1">
-        <v>0.03</v>
+      <c r="C37" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1950</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>0.01</v>
       </c>
-      <c r="C38" s="1">
-        <v>0.03</v>
+      <c r="C38" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1951</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>0.08</v>
       </c>
-      <c r="C39" s="1">
-        <v>0.03</v>
+      <c r="C39" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1952</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>0.02</v>
       </c>
-      <c r="C40" s="1">
-        <v>0.03</v>
+      <c r="C40" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1953</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>0.01</v>
       </c>
-      <c r="C41" s="1">
-        <v>0.03</v>
+      <c r="C41" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1954</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>0.01</v>
       </c>
-      <c r="C42" s="1">
-        <v>0.03</v>
+      <c r="C42" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1955</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>0</v>
       </c>
-      <c r="C43" s="1">
-        <v>0.03</v>
+      <c r="C43" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1956</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>0.02</v>
       </c>
-      <c r="C44" s="1">
-        <v>0.03</v>
+      <c r="C44" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1957</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>0.03</v>
       </c>
-      <c r="C45" s="1">
-        <v>0.03</v>
+      <c r="C45" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1958</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>0.03</v>
       </c>
-      <c r="C46" s="1">
-        <v>0.03</v>
+      <c r="C46" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1959</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>0.01</v>
       </c>
-      <c r="C47" s="1">
-        <v>0.03</v>
+      <c r="C47" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1960</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>0.02</v>
       </c>
-      <c r="C48" s="1">
-        <v>0.03</v>
+      <c r="C48" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1961</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>0.01</v>
       </c>
-      <c r="C49" s="1">
-        <v>0.03</v>
+      <c r="C49" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1962</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>0.01</v>
       </c>
-      <c r="C50" s="1">
-        <v>0.03</v>
+      <c r="C50" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1963</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>0.01</v>
       </c>
-      <c r="C51" s="1">
-        <v>0.03</v>
+      <c r="C51" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1964</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>0.01</v>
       </c>
-      <c r="C52" s="1">
-        <v>0.03</v>
+      <c r="C52" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1965</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>0.02</v>
       </c>
-      <c r="C53" s="1">
-        <v>0.03</v>
+      <c r="C53" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1966</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>0.03</v>
       </c>
-      <c r="C54" s="1">
-        <v>0.03</v>
+      <c r="C54" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1967</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>0.03</v>
       </c>
-      <c r="C55" s="1">
-        <v>0.03</v>
+      <c r="C55" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1968</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>0.04</v>
       </c>
-      <c r="C56" s="1">
-        <v>0.03</v>
+      <c r="C56" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1969</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>0.06</v>
       </c>
-      <c r="C57" s="1">
-        <v>0.03</v>
+      <c r="C57" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1970</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>0.06</v>
       </c>
-      <c r="C58" s="1">
-        <v>0.03</v>
+      <c r="C58" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1971</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>0.04</v>
       </c>
-      <c r="C59" s="1">
-        <v>0.03</v>
+      <c r="C59" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1972</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>0.03</v>
       </c>
-      <c r="C60" s="1">
-        <v>0.03</v>
+      <c r="C60" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1973</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>0.06</v>
       </c>
-      <c r="C61" s="1">
-        <v>0.03</v>
+      <c r="C61" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1974</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>0.11</v>
       </c>
-      <c r="C62" s="1">
-        <v>0.03</v>
+      <c r="C62" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1975</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>0.09</v>
       </c>
-      <c r="C63" s="1">
-        <v>0.03</v>
+      <c r="C63" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1976</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>0.06</v>
       </c>
-      <c r="C64" s="1">
-        <v>0.03</v>
+      <c r="C64" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1977</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C65" s="1">
-        <v>0.03</v>
+      <c r="C65" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1978</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>0.08</v>
       </c>
-      <c r="C66" s="1">
-        <v>0.03</v>
+      <c r="C66" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1979</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>0.11</v>
       </c>
-      <c r="C67" s="1">
-        <v>0.03</v>
+      <c r="C67" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1980</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C68" s="1">
-        <v>0.03</v>
+      <c r="C68" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1981</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>0.1</v>
       </c>
-      <c r="C69" s="1">
-        <v>0.03</v>
+      <c r="C69" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1982</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>0.06</v>
       </c>
-      <c r="C70" s="1">
-        <v>0.03</v>
+      <c r="C70" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1983</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>0.03</v>
       </c>
-      <c r="C71" s="1">
-        <v>0.03</v>
+      <c r="C71" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1984</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>0.04</v>
       </c>
-      <c r="C72" s="1">
-        <v>0.03</v>
+      <c r="C72" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1985</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>0.04</v>
       </c>
-      <c r="C73" s="1">
-        <v>0.03</v>
+      <c r="C73" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1986</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>0.02</v>
       </c>
-      <c r="C74" s="1">
-        <v>0.03</v>
+      <c r="C74" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1987</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>0.04</v>
       </c>
-      <c r="C75" s="1">
-        <v>0.03</v>
+      <c r="C75" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1988</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>0.04</v>
       </c>
-      <c r="C76" s="1">
-        <v>0.03</v>
+      <c r="C76" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1989</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>0.05</v>
       </c>
-      <c r="C77" s="1">
-        <v>0.03</v>
+      <c r="C77" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1990</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>0.05</v>
       </c>
-      <c r="C78" s="1">
-        <v>0.03</v>
+      <c r="C78" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1991</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>0.04</v>
       </c>
-      <c r="C79" s="1">
-        <v>0.03</v>
+      <c r="C79" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1992</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>0.03</v>
       </c>
-      <c r="C80" s="1">
-        <v>0.03</v>
+      <c r="C80" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1993</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>0.03</v>
       </c>
-      <c r="C81" s="1">
-        <v>0.03</v>
+      <c r="C81" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1994</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>0.03</v>
       </c>
-      <c r="C82" s="1">
-        <v>0.03</v>
+      <c r="C82" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1995</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>0.03</v>
       </c>
-      <c r="C83" s="1">
-        <v>0.03</v>
+      <c r="C83" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1996</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="1">
         <v>0.03</v>
       </c>
-      <c r="C84" s="1">
-        <v>0.03</v>
+      <c r="C84" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1997</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="1">
         <v>0.02</v>
       </c>
-      <c r="C85" s="1">
-        <v>0.03</v>
+      <c r="C85" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1998</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>0.02</v>
       </c>
-      <c r="C86" s="1">
-        <v>0.03</v>
+      <c r="C86" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1999</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>0.02</v>
       </c>
-      <c r="C87" s="1">
-        <v>0.03</v>
+      <c r="C87" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2000</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>0.03</v>
       </c>
-      <c r="C88" s="1">
-        <v>0.03</v>
+      <c r="C88" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2001</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>0.03</v>
       </c>
-      <c r="C89" s="1">
-        <v>0.03</v>
+      <c r="C89" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2002</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>0.02</v>
       </c>
-      <c r="C90" s="1">
-        <v>0.03</v>
+      <c r="C90" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2003</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>0.02</v>
       </c>
-      <c r="C91" s="1">
-        <v>0.03</v>
+      <c r="C91" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2004</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>0.03</v>
       </c>
-      <c r="C92" s="1">
-        <v>0.03</v>
+      <c r="C92" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2005</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>0.03</v>
       </c>
-      <c r="C93" s="1">
-        <v>0.03</v>
+      <c r="C93" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2006</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>0.03</v>
       </c>
-      <c r="C94" s="1">
-        <v>0.03</v>
+      <c r="C94" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2007</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="1">
         <v>0.03</v>
       </c>
-      <c r="C95" s="1">
-        <v>0.03</v>
+      <c r="C95" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2008</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="1">
         <v>0.04</v>
       </c>
-      <c r="C96" s="1">
-        <v>0.03</v>
+      <c r="C96" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2009</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="1">
         <v>0</v>
       </c>
-      <c r="C97" s="1">
-        <v>0.03</v>
+      <c r="C97" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2010</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="1">
         <v>0.02</v>
       </c>
-      <c r="C98" s="1">
-        <v>0.03</v>
+      <c r="C98" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2011</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="1">
         <v>0.03</v>
       </c>
-      <c r="C99" s="1">
-        <v>0.03</v>
+      <c r="C99" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2012</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="1">
         <v>0.02</v>
       </c>
-      <c r="C100" s="1">
-        <v>0.03</v>
+      <c r="C100" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2013</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="1">
         <v>0.02</v>
       </c>
-      <c r="C101" s="1">
-        <v>0.03</v>
+      <c r="C101" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2014</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102" s="1">
         <v>0.02</v>
       </c>
-      <c r="C102" s="1">
-        <v>0.03</v>
+      <c r="C102" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2015</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103" s="1">
         <v>0</v>
       </c>
-      <c r="C103" s="1">
-        <v>0.03</v>
+      <c r="C103" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2016</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104" s="1">
         <v>0.01</v>
       </c>
-      <c r="C104" s="1">
-        <v>0.03</v>
+      <c r="C104" s="3">
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>